<commit_message>
fix(module) : template 替换
template 替换
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -11,18 +11,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="29">
-  <si>
-    <t>锐石前端周报（3月）</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="26">
+  <si>
+    <t>position周报（3月）</t>
   </si>
   <si>
     <t>日期：2018年3月14日-2018年3月16日</t>
   </si>
   <si>
-    <t>职位：前端开发</t>
-  </si>
-  <si>
-    <t>姓名：张煜</t>
+    <t>职位：position</t>
+  </si>
+  <si>
+    <t>姓名：name</t>
   </si>
   <si>
     <t>本周工作总结</t>
@@ -73,19 +73,10 @@
     <t>星期三</t>
   </si>
   <si>
-    <t>项目接收,优化项目,压缩代码量</t>
-  </si>
-  <si>
     <t>星期四</t>
   </si>
   <si>
-    <t>项产品理解项目的运行</t>
-  </si>
-  <si>
     <t>星期五</t>
-  </si>
-  <si>
-    <t>亚盘的补单样式添加,数据接入</t>
   </si>
   <si>
     <t>下周工作计划</t>
@@ -624,17 +615,17 @@
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -662,10 +653,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -913,12 +904,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1205,7 +1196,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1233,10 +1224,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1683,9 +1674,7 @@
       <c r="B12" s="20">
         <v>43173</v>
       </c>
-      <c r="C12" t="s" s="22">
-        <v>20</v>
-      </c>
+      <c r="C12" s="22"/>
       <c r="D12" s="14">
         <v>3</v>
       </c>
@@ -1696,14 +1685,12 @@
     </row>
     <row r="13" ht="51.75" customHeight="1">
       <c r="A13" t="s" s="19">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13" s="20">
         <v>43174</v>
       </c>
-      <c r="C13" t="s" s="22">
-        <v>22</v>
-      </c>
+      <c r="C13" s="22"/>
       <c r="D13" s="23"/>
       <c r="E13" s="21"/>
       <c r="F13" s="21"/>
@@ -1712,14 +1699,12 @@
     </row>
     <row r="14" ht="59.25" customHeight="1">
       <c r="A14" t="s" s="19">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B14" s="20">
         <v>43175</v>
       </c>
-      <c r="C14" t="s" s="22">
-        <v>24</v>
-      </c>
+      <c r="C14" s="22"/>
       <c r="D14" s="23"/>
       <c r="E14" s="21"/>
       <c r="F14" s="21"/>
@@ -1728,7 +1713,7 @@
     </row>
     <row r="15" ht="26" customHeight="1">
       <c r="A15" t="s" s="8">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B15" s="9"/>
       <c r="C15" s="9"/>
@@ -1760,7 +1745,7 @@
         <v>43115</v>
       </c>
       <c r="C17" t="s" s="24">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D17" s="25"/>
       <c r="E17" s="25"/>
@@ -1776,7 +1761,7 @@
         <v>43116</v>
       </c>
       <c r="C18" t="s" s="24">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D18" s="25"/>
       <c r="E18" s="25"/>
@@ -1792,7 +1777,7 @@
         <v>43117</v>
       </c>
       <c r="C19" t="s" s="24">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D19" s="25"/>
       <c r="E19" s="25"/>
@@ -1802,13 +1787,13 @@
     </row>
     <row r="20" ht="53.25" customHeight="1">
       <c r="A20" t="s" s="19">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B20" s="20">
         <v>43118</v>
       </c>
       <c r="C20" t="s" s="24">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D20" s="25"/>
       <c r="E20" s="25"/>
@@ -1818,13 +1803,13 @@
     </row>
     <row r="21" ht="49.5" customHeight="1">
       <c r="A21" t="s" s="19">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B21" s="20">
         <v>43119</v>
       </c>
       <c r="C21" t="s" s="24">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D21" s="25"/>
       <c r="E21" s="25"/>
@@ -1834,7 +1819,7 @@
     </row>
     <row r="22" ht="30.75" customHeight="1">
       <c r="A22" t="s" s="19">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B22" s="23"/>
       <c r="C22" s="27"/>
@@ -1846,7 +1831,7 @@
     </row>
     <row r="23" ht="98.25" customHeight="1">
       <c r="A23" t="s" s="28">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B23" s="29"/>
       <c r="C23" s="29"/>
@@ -1858,33 +1843,33 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="A15:F15"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="C17:F17"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="A23:F23"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="C22:F22"/>
+    <mergeCell ref="C19:F19"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="C18:F18"/>
+    <mergeCell ref="C21:F21"/>
     <mergeCell ref="C20:F20"/>
-    <mergeCell ref="C21:F21"/>
-    <mergeCell ref="C19:F19"/>
-    <mergeCell ref="C18:F18"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="C22:F22"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="A23:F23"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="C17:F17"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="C16:F16"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="A15:F15"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="B6:C6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>

<commit_message>
feat(module) :  读取 Excel
尝试读取 Excel
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -5,7 +5,7 @@
     <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
   </bookViews>
   <sheets>
-    <sheet name="工作表1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
 </workbook>
 </file>
@@ -1843,33 +1843,33 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="C20:F20"/>
+    <mergeCell ref="C21:F21"/>
+    <mergeCell ref="C18:F18"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="C19:F19"/>
+    <mergeCell ref="C22:F22"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="A23:F23"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="C17:F17"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="E6:F6"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="E5:F5"/>
+    <mergeCell ref="A15:F15"/>
     <mergeCell ref="D3:F3"/>
-    <mergeCell ref="A15:F15"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="C16:F16"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="C17:F17"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="A23:F23"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="C22:F22"/>
-    <mergeCell ref="C19:F19"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="C18:F18"/>
-    <mergeCell ref="C21:F21"/>
-    <mergeCell ref="C20:F20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>

<commit_message>
#     样式 :    feat(location): 接入登录API # #                  登录功能与服务器对接 #
test(location) :  test style

<body>

<footer>

#其中 type 的值可以有
#    .feat :新功能 
#    .fix :修复bug
#    .doc :文档改变
#    .style :代码格式改变
#    .refactor :某个已有功能重构
#    .perf :性能优化
#    .test :增加测试
#    .build :改变了build工具 如 grunt换成了 npm
#    .revert :撤销上一次的 commit 
#
#scope :用来说明此次修改的影响范围
#     .all :表示影响面大 ，如修改了网络框架  会对真个程序产生影响
#     .loation :表示影响小，某个小小的功能
#     .module :表示会影响某个模块 如登录模块、首页模块 、用户管理模块等等
#
#subject: 用来简要描述本次改动，概述就好了
# 
#body :具体的修改信息 应该尽量详细
# 
#footer :放置写备注啥的，如果是 bug ，可以把bug id放入
#
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -144,7 +144,7 @@
       <name val="微软雅黑"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -165,12 +165,24 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor indexed="11"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor indexed="12"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -198,67 +210,7 @@
         <color indexed="8"/>
       </left>
       <right style="thin">
-        <color indexed="11"/>
-      </right>
-      <top style="thin">
-        <color indexed="11"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="11"/>
-      </left>
-      <right style="thin">
-        <color indexed="11"/>
-      </right>
-      <top style="thin">
-        <color indexed="11"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="13"/>
-      </right>
-      <top style="thin">
-        <color indexed="11"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="13"/>
-      </left>
-      <right style="thin">
-        <color indexed="11"/>
-      </right>
-      <top style="thin">
-        <color indexed="11"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="11"/>
+        <color indexed="14"/>
       </right>
       <top style="thin">
         <color indexed="8"/>
@@ -270,10 +222,10 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="11"/>
+        <color indexed="14"/>
       </left>
       <right style="thin">
-        <color indexed="11"/>
+        <color indexed="14"/>
       </right>
       <top style="thin">
         <color indexed="8"/>
@@ -285,7 +237,7 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="11"/>
+        <color indexed="14"/>
       </left>
       <right style="thin">
         <color indexed="8"/>
@@ -304,7 +256,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -314,82 +266,73 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="5" fillId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="7" fillId="6" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="5" fillId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="56" fontId="7" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="56" fontId="7" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="7" fillId="6" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="6" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -412,11 +355,12 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="fff6be98"/>
       <rgbColor rgb="ffa9cd90"/>
+      <rgbColor rgb="fff7caac"/>
+      <rgbColor rgb="ff93c175"/>
       <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
-      <rgbColor rgb="fff7caac"/>
-      <rgbColor rgb="ff70ad47"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1478,7 +1422,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1490,9 +1434,7 @@
     <col min="4" max="4" width="11.6719" style="1" customWidth="1"/>
     <col min="5" max="5" width="29.1719" style="1" customWidth="1"/>
     <col min="6" max="6" width="35.1719" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11" style="1" customWidth="1"/>
-    <col min="8" max="8" width="11" style="1" customWidth="1"/>
-    <col min="9" max="256" width="11" style="1" customWidth="1"/>
+    <col min="7" max="256" width="11" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="43" customHeight="1">
@@ -1504,372 +1446,326 @@
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="5"/>
     </row>
     <row r="2" ht="32" customHeight="1">
-      <c r="A2" t="s" s="6">
+      <c r="A2" t="s" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" t="s" s="6">
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" t="s" s="4">
         <v>2</v>
       </c>
-      <c r="E2" s="7"/>
-      <c r="F2" t="s" s="6">
+      <c r="E2" s="5"/>
+      <c r="F2" t="s" s="4">
         <v>3</v>
       </c>
-      <c r="G2" s="4"/>
-      <c r="H2" s="5"/>
     </row>
     <row r="3" ht="32" customHeight="1">
-      <c r="A3" t="s" s="8">
+      <c r="A3" t="s" s="6">
         <v>4</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" t="s" s="8">
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" t="s" s="6">
         <v>5</v>
       </c>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="5"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
     </row>
     <row r="4" ht="26" customHeight="1">
-      <c r="A4" t="s" s="10">
+      <c r="A4" t="s" s="8">
         <v>6</v>
       </c>
-      <c r="B4" t="s" s="10">
+      <c r="B4" t="s" s="8">
         <v>7</v>
       </c>
-      <c r="C4" s="11"/>
-      <c r="D4" t="s" s="10">
+      <c r="C4" s="9"/>
+      <c r="D4" t="s" s="8">
         <v>6</v>
       </c>
-      <c r="E4" t="s" s="10">
+      <c r="E4" t="s" s="8">
         <v>8</v>
       </c>
-      <c r="F4" s="11"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="13"/>
+      <c r="F4" s="9"/>
     </row>
     <row r="5" ht="31" customHeight="1">
-      <c r="A5" s="14">
+      <c r="A5" s="10">
         <v>1</v>
       </c>
-      <c r="B5" t="s" s="15">
+      <c r="B5" t="s" s="11">
         <v>9</v>
       </c>
-      <c r="C5" s="16"/>
-      <c r="D5" s="14">
+      <c r="C5" s="12"/>
+      <c r="D5" s="10">
         <v>1</v>
       </c>
-      <c r="E5" t="s" s="15">
+      <c r="E5" t="s" s="11">
         <v>9</v>
       </c>
-      <c r="F5" s="16"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="5"/>
+      <c r="F5" s="12"/>
     </row>
     <row r="6" ht="31" customHeight="1">
-      <c r="A6" s="14">
+      <c r="A6" s="10">
         <v>2</v>
       </c>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="14">
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="10">
         <v>2</v>
       </c>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="5"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
     </row>
     <row r="7" ht="31" customHeight="1">
-      <c r="A7" s="14">
+      <c r="A7" s="10">
         <v>3</v>
       </c>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="14">
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="10">
         <v>3</v>
       </c>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="5"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
     </row>
     <row r="8" ht="26" customHeight="1">
-      <c r="A8" t="s" s="17">
+      <c r="A8" t="s" s="13">
         <v>10</v>
       </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" t="s" s="8">
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" t="s" s="6">
         <v>11</v>
       </c>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="5"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
     </row>
     <row r="9" ht="23" customHeight="1">
-      <c r="A9" t="s" s="10">
+      <c r="A9" t="s" s="8">
         <v>12</v>
       </c>
-      <c r="B9" s="11"/>
-      <c r="C9" t="s" s="10">
+      <c r="B9" s="9"/>
+      <c r="C9" t="s" s="8">
         <v>13</v>
       </c>
-      <c r="D9" t="s" s="10">
+      <c r="D9" t="s" s="8">
         <v>14</v>
       </c>
-      <c r="E9" t="s" s="10">
+      <c r="E9" t="s" s="8">
         <v>15</v>
       </c>
-      <c r="F9" t="s" s="10">
+      <c r="F9" t="s" s="8">
         <v>16</v>
       </c>
-      <c r="G9" s="4"/>
-      <c r="H9" s="5"/>
     </row>
     <row r="10" ht="62.25" customHeight="1">
-      <c r="A10" t="s" s="19">
+      <c r="A10" t="s" s="15">
         <v>17</v>
       </c>
-      <c r="B10" s="20">
+      <c r="B10" s="16">
         <v>43171</v>
       </c>
-      <c r="C10" s="21"/>
-      <c r="D10" s="14">
+      <c r="C10" s="17"/>
+      <c r="D10" s="10">
         <v>1</v>
       </c>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="5"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
     </row>
     <row r="11" ht="59.25" customHeight="1">
-      <c r="A11" t="s" s="19">
+      <c r="A11" t="s" s="15">
         <v>18</v>
       </c>
-      <c r="B11" s="20">
+      <c r="B11" s="16">
         <v>43172</v>
       </c>
-      <c r="C11" s="21"/>
-      <c r="D11" s="14">
+      <c r="C11" s="17"/>
+      <c r="D11" s="10">
         <v>2</v>
       </c>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="5"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
     </row>
     <row r="12" ht="51.75" customHeight="1">
-      <c r="A12" t="s" s="19">
+      <c r="A12" t="s" s="15">
         <v>19</v>
       </c>
-      <c r="B12" s="20">
+      <c r="B12" s="16">
         <v>43173</v>
       </c>
-      <c r="C12" s="22"/>
-      <c r="D12" s="14">
+      <c r="C12" s="18"/>
+      <c r="D12" s="10">
         <v>3</v>
       </c>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="5"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
     </row>
     <row r="13" ht="51.75" customHeight="1">
-      <c r="A13" t="s" s="19">
+      <c r="A13" t="s" s="15">
         <v>20</v>
       </c>
-      <c r="B13" s="20">
+      <c r="B13" s="16">
         <v>43174</v>
       </c>
-      <c r="C13" s="22"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="5"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
     </row>
     <row r="14" ht="59.25" customHeight="1">
-      <c r="A14" t="s" s="19">
+      <c r="A14" t="s" s="15">
         <v>21</v>
       </c>
-      <c r="B14" s="20">
+      <c r="B14" s="16">
         <v>43175</v>
       </c>
-      <c r="C14" s="22"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="5"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
     </row>
     <row r="15" ht="26" customHeight="1">
-      <c r="A15" t="s" s="8">
+      <c r="A15" t="s" s="6">
         <v>22</v>
       </c>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="5"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
     </row>
     <row r="16" ht="30" customHeight="1">
-      <c r="A16" t="s" s="10">
+      <c r="A16" t="s" s="8">
         <v>12</v>
       </c>
-      <c r="B16" s="11"/>
-      <c r="C16" t="s" s="10">
+      <c r="B16" s="9"/>
+      <c r="C16" t="s" s="8">
         <v>13</v>
       </c>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="5"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
     </row>
     <row r="17" ht="57" customHeight="1">
-      <c r="A17" t="s" s="19">
+      <c r="A17" t="s" s="15">
         <v>17</v>
       </c>
-      <c r="B17" s="20">
+      <c r="B17" s="16">
         <v>43115</v>
       </c>
-      <c r="C17" t="s" s="24">
+      <c r="C17" t="s" s="20">
         <v>23</v>
       </c>
-      <c r="D17" s="25"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="26"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="5"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="22"/>
     </row>
     <row r="18" ht="51" customHeight="1">
-      <c r="A18" t="s" s="19">
+      <c r="A18" t="s" s="15">
         <v>18</v>
       </c>
-      <c r="B18" s="20">
+      <c r="B18" s="16">
         <v>43116</v>
       </c>
-      <c r="C18" t="s" s="24">
+      <c r="C18" t="s" s="20">
         <v>23</v>
       </c>
-      <c r="D18" s="25"/>
-      <c r="E18" s="25"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="5"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="22"/>
     </row>
     <row r="19" ht="53.25" customHeight="1">
-      <c r="A19" t="s" s="19">
+      <c r="A19" t="s" s="15">
         <v>19</v>
       </c>
-      <c r="B19" s="20">
+      <c r="B19" s="16">
         <v>43117</v>
       </c>
-      <c r="C19" t="s" s="24">
+      <c r="C19" t="s" s="20">
         <v>23</v>
       </c>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="26"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="5"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="22"/>
     </row>
     <row r="20" ht="53.25" customHeight="1">
-      <c r="A20" t="s" s="19">
+      <c r="A20" t="s" s="15">
         <v>20</v>
       </c>
-      <c r="B20" s="20">
+      <c r="B20" s="16">
         <v>43118</v>
       </c>
-      <c r="C20" t="s" s="24">
+      <c r="C20" t="s" s="20">
         <v>23</v>
       </c>
-      <c r="D20" s="25"/>
-      <c r="E20" s="25"/>
-      <c r="F20" s="26"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="5"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="22"/>
     </row>
     <row r="21" ht="49.5" customHeight="1">
-      <c r="A21" t="s" s="19">
+      <c r="A21" t="s" s="15">
         <v>21</v>
       </c>
-      <c r="B21" s="20">
+      <c r="B21" s="16">
         <v>43119</v>
       </c>
-      <c r="C21" t="s" s="24">
+      <c r="C21" t="s" s="20">
         <v>23</v>
       </c>
-      <c r="D21" s="25"/>
-      <c r="E21" s="25"/>
-      <c r="F21" s="26"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="5"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="22"/>
     </row>
     <row r="22" ht="30.75" customHeight="1">
-      <c r="A22" t="s" s="19">
+      <c r="A22" t="s" s="15">
         <v>24</v>
       </c>
       <c r="B22" s="23"/>
-      <c r="C22" s="27"/>
-      <c r="D22" s="25"/>
-      <c r="E22" s="25"/>
-      <c r="F22" s="26"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="5"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="22"/>
     </row>
     <row r="23" ht="98.25" customHeight="1">
-      <c r="A23" t="s" s="28">
+      <c r="A23" t="s" s="25">
         <v>25</v>
       </c>
-      <c r="B23" s="29"/>
-      <c r="C23" s="29"/>
-      <c r="D23" s="29"/>
-      <c r="E23" s="29"/>
-      <c r="F23" s="29"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="5"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="26"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="C20:F20"/>
-    <mergeCell ref="C21:F21"/>
-    <mergeCell ref="C18:F18"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="C19:F19"/>
-    <mergeCell ref="C22:F22"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="A23:F23"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="C17:F17"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="C16:F16"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="A15:F15"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="E5:F5"/>
-    <mergeCell ref="A15:F15"/>
-    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="A23:F23"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="C22:F22"/>
+    <mergeCell ref="C19:F19"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="C18:F18"/>
+    <mergeCell ref="C21:F21"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="C17:F17"/>
+    <mergeCell ref="C20:F20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>

<commit_message>
feat(location) : str replace
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -11,18 +11,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="26">
-  <si>
-    <t>position周报（3月）</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="31">
+  <si>
+    <t>{position}周报（{month}月）</t>
   </si>
   <si>
     <t>日期：2018年3月14日-2018年3月16日</t>
   </si>
   <si>
-    <t>职位：position</t>
-  </si>
-  <si>
-    <t>姓名：name</t>
+    <t>职位：{position}</t>
+  </si>
+  <si>
+    <t>姓名：{name}</t>
   </si>
   <si>
     <t>本周工作总结</t>
@@ -40,7 +40,22 @@
     <t>下周主要事项</t>
   </si>
   <si>
-    <t>新项目开发</t>
+    <t>{maindo1}</t>
+  </si>
+  <si>
+    <t>{maintodo1}</t>
+  </si>
+  <si>
+    <t>{maindo2}</t>
+  </si>
+  <si>
+    <t>{maintodo2}</t>
+  </si>
+  <si>
+    <t>{maindo3}</t>
+  </si>
+  <si>
+    <t>{maintodo3}</t>
   </si>
   <si>
     <t>本周工作记录</t>
@@ -1501,7 +1516,7 @@
         <v>1</v>
       </c>
       <c r="E5" t="s" s="11">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F5" s="12"/>
     </row>
@@ -1509,59 +1524,67 @@
       <c r="A6" s="10">
         <v>2</v>
       </c>
-      <c r="B6" s="12"/>
+      <c r="B6" t="s" s="11">
+        <v>11</v>
+      </c>
       <c r="C6" s="12"/>
       <c r="D6" s="10">
         <v>2</v>
       </c>
-      <c r="E6" s="12"/>
+      <c r="E6" t="s" s="11">
+        <v>12</v>
+      </c>
       <c r="F6" s="12"/>
     </row>
     <row r="7" ht="31" customHeight="1">
       <c r="A7" s="10">
         <v>3</v>
       </c>
-      <c r="B7" s="12"/>
+      <c r="B7" t="s" s="11">
+        <v>13</v>
+      </c>
       <c r="C7" s="12"/>
       <c r="D7" s="10">
         <v>3</v>
       </c>
-      <c r="E7" s="12"/>
+      <c r="E7" t="s" s="11">
+        <v>14</v>
+      </c>
       <c r="F7" s="12"/>
     </row>
     <row r="8" ht="26" customHeight="1">
       <c r="A8" t="s" s="13">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B8" s="14"/>
       <c r="C8" s="14"/>
       <c r="D8" t="s" s="6">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
     </row>
     <row r="9" ht="23" customHeight="1">
       <c r="A9" t="s" s="8">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B9" s="9"/>
       <c r="C9" t="s" s="8">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D9" t="s" s="8">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="E9" t="s" s="8">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="F9" t="s" s="8">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" ht="62.25" customHeight="1">
       <c r="A10" t="s" s="15">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B10" s="16">
         <v>43171</v>
@@ -1575,7 +1598,7 @@
     </row>
     <row r="11" ht="59.25" customHeight="1">
       <c r="A11" t="s" s="15">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B11" s="16">
         <v>43172</v>
@@ -1589,7 +1612,7 @@
     </row>
     <row r="12" ht="51.75" customHeight="1">
       <c r="A12" t="s" s="15">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B12" s="16">
         <v>43173</v>
@@ -1603,7 +1626,7 @@
     </row>
     <row r="13" ht="51.75" customHeight="1">
       <c r="A13" t="s" s="15">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B13" s="16">
         <v>43174</v>
@@ -1615,7 +1638,7 @@
     </row>
     <row r="14" ht="59.25" customHeight="1">
       <c r="A14" t="s" s="15">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="B14" s="16">
         <v>43175</v>
@@ -1627,7 +1650,7 @@
     </row>
     <row r="15" ht="26" customHeight="1">
       <c r="A15" t="s" s="6">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
@@ -1637,11 +1660,11 @@
     </row>
     <row r="16" ht="30" customHeight="1">
       <c r="A16" t="s" s="8">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B16" s="9"/>
       <c r="C16" t="s" s="8">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D16" s="9"/>
       <c r="E16" s="9"/>
@@ -1649,13 +1672,13 @@
     </row>
     <row r="17" ht="57" customHeight="1">
       <c r="A17" t="s" s="15">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B17" s="16">
         <v>43115</v>
       </c>
       <c r="C17" t="s" s="20">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="D17" s="21"/>
       <c r="E17" s="21"/>
@@ -1663,13 +1686,13 @@
     </row>
     <row r="18" ht="51" customHeight="1">
       <c r="A18" t="s" s="15">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B18" s="16">
         <v>43116</v>
       </c>
       <c r="C18" t="s" s="20">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="D18" s="21"/>
       <c r="E18" s="21"/>
@@ -1677,13 +1700,13 @@
     </row>
     <row r="19" ht="53.25" customHeight="1">
       <c r="A19" t="s" s="15">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B19" s="16">
         <v>43117</v>
       </c>
       <c r="C19" t="s" s="20">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="D19" s="21"/>
       <c r="E19" s="21"/>
@@ -1691,13 +1714,13 @@
     </row>
     <row r="20" ht="53.25" customHeight="1">
       <c r="A20" t="s" s="15">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B20" s="16">
         <v>43118</v>
       </c>
       <c r="C20" t="s" s="20">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="D20" s="21"/>
       <c r="E20" s="21"/>
@@ -1705,13 +1728,13 @@
     </row>
     <row r="21" ht="49.5" customHeight="1">
       <c r="A21" t="s" s="15">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="B21" s="16">
         <v>43119</v>
       </c>
       <c r="C21" t="s" s="20">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="D21" s="21"/>
       <c r="E21" s="21"/>
@@ -1719,7 +1742,7 @@
     </row>
     <row r="22" ht="30.75" customHeight="1">
       <c r="A22" t="s" s="15">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B22" s="23"/>
       <c r="C22" s="24"/>
@@ -1729,7 +1752,7 @@
     </row>
     <row r="23" ht="98.25" customHeight="1">
       <c r="A23" t="s" s="25">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B23" s="26"/>
       <c r="C23" s="26"/>

</xml_diff>

<commit_message>
feat(module) : get timeList
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -11,12 +11,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="46">
   <si>
     <t>{position}周报（{month}月）</t>
   </si>
   <si>
-    <t>日期：2018年3月14日-2018年3月16日</t>
+    <t>日期：{thisWeekStr}</t>
   </si>
   <si>
     <t>职位：{position}</t>
@@ -79,25 +79,81 @@
     <t>提议解决办法</t>
   </si>
   <si>
-    <t>星期一</t>
-  </si>
-  <si>
-    <t>星期二</t>
-  </si>
-  <si>
-    <t>星期三</t>
-  </si>
-  <si>
-    <t>星期四</t>
-  </si>
-  <si>
-    <t>星期五</t>
+    <t xml:space="preserve">{thisWeek.Mon}
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{thisWeek.MonDate}
+</t>
+  </si>
+  <si>
+    <t>{thisWeek.Tues}</t>
+  </si>
+  <si>
+    <t>{thisWeek.TuesDate}</t>
+  </si>
+  <si>
+    <t>{thisWeek.Wed}</t>
+  </si>
+  <si>
+    <t>{thisWeek.WedDate}</t>
+  </si>
+  <si>
+    <t>{thisWeek.Thur}</t>
+  </si>
+  <si>
+    <t>{thisWeek.ThurDate}</t>
+  </si>
+  <si>
+    <t>{thisWeek.Fri}</t>
+  </si>
+  <si>
+    <t>{thisWeek.FriDate}</t>
   </si>
   <si>
     <t>下周工作计划</t>
   </si>
   <si>
+    <t xml:space="preserve">{nextWeek.Mon}
+</t>
+  </si>
+  <si>
+    <t>{nextWeek.MonDate}</t>
+  </si>
+  <si>
     <t>新项目后台数据及逻辑交互</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{nextWeek.Thes}
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{nextWeek.ThesDate}
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{nextWeek.Wed}
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{nextWeek.WedDate}
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{nextWeek.Thur}
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{nextWeek.ThurDate}
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{nextWeek.Fri}
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{nextWeek.FriDate}
+</t>
   </si>
   <si>
     <t>额外工作说明</t>
@@ -271,7 +327,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -312,9 +368,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="56" fontId="7" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1574,8 +1627,8 @@
       <c r="A10" t="s" s="13">
         <v>22</v>
       </c>
-      <c r="B10" s="14">
-        <v>43171</v>
+      <c r="B10" t="s" s="13">
+        <v>23</v>
       </c>
       <c r="C10" s="12"/>
       <c r="D10" s="10">
@@ -1586,10 +1639,10 @@
     </row>
     <row r="11" ht="59.25" customHeight="1">
       <c r="A11" t="s" s="13">
-        <v>23</v>
-      </c>
-      <c r="B11" s="14">
-        <v>43172</v>
+        <v>24</v>
+      </c>
+      <c r="B11" t="s" s="13">
+        <v>25</v>
       </c>
       <c r="C11" s="12"/>
       <c r="D11" s="10">
@@ -1600,12 +1653,12 @@
     </row>
     <row r="12" ht="51.75" customHeight="1">
       <c r="A12" t="s" s="13">
-        <v>24</v>
-      </c>
-      <c r="B12" s="14">
-        <v>43173</v>
-      </c>
-      <c r="C12" s="11"/>
+        <v>26</v>
+      </c>
+      <c r="B12" t="s" s="13">
+        <v>27</v>
+      </c>
+      <c r="C12" s="12"/>
       <c r="D12" s="10">
         <v>3</v>
       </c>
@@ -1614,31 +1667,31 @@
     </row>
     <row r="13" ht="51.75" customHeight="1">
       <c r="A13" t="s" s="13">
-        <v>25</v>
-      </c>
-      <c r="B13" s="14">
-        <v>43174</v>
-      </c>
-      <c r="C13" s="11"/>
-      <c r="D13" s="15"/>
+        <v>28</v>
+      </c>
+      <c r="B13" t="s" s="13">
+        <v>29</v>
+      </c>
+      <c r="C13" s="12"/>
+      <c r="D13" s="14"/>
       <c r="E13" s="12"/>
       <c r="F13" s="12"/>
     </row>
     <row r="14" ht="59.25" customHeight="1">
       <c r="A14" t="s" s="13">
-        <v>26</v>
-      </c>
-      <c r="B14" s="14">
-        <v>43175</v>
-      </c>
-      <c r="C14" s="11"/>
-      <c r="D14" s="15"/>
+        <v>30</v>
+      </c>
+      <c r="B14" t="s" s="13">
+        <v>31</v>
+      </c>
+      <c r="C14" s="12"/>
+      <c r="D14" s="14"/>
       <c r="E14" s="12"/>
       <c r="F14" s="12"/>
     </row>
     <row r="15" ht="26" customHeight="1">
       <c r="A15" t="s" s="6">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
@@ -1660,93 +1713,93 @@
     </row>
     <row r="17" ht="57" customHeight="1">
       <c r="A17" t="s" s="13">
-        <v>22</v>
-      </c>
-      <c r="B17" s="14">
-        <v>43115</v>
-      </c>
-      <c r="C17" t="s" s="16">
-        <v>28</v>
-      </c>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="18"/>
+        <v>33</v>
+      </c>
+      <c r="B17" t="s" s="13">
+        <v>34</v>
+      </c>
+      <c r="C17" t="s" s="15">
+        <v>35</v>
+      </c>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="17"/>
     </row>
     <row r="18" ht="51" customHeight="1">
       <c r="A18" t="s" s="13">
-        <v>23</v>
-      </c>
-      <c r="B18" s="14">
-        <v>43116</v>
-      </c>
-      <c r="C18" t="s" s="16">
-        <v>28</v>
-      </c>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="18"/>
+        <v>36</v>
+      </c>
+      <c r="B18" t="s" s="13">
+        <v>37</v>
+      </c>
+      <c r="C18" t="s" s="15">
+        <v>35</v>
+      </c>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="17"/>
     </row>
     <row r="19" ht="53.25" customHeight="1">
       <c r="A19" t="s" s="13">
-        <v>24</v>
-      </c>
-      <c r="B19" s="14">
-        <v>43117</v>
-      </c>
-      <c r="C19" t="s" s="16">
-        <v>28</v>
-      </c>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="18"/>
+        <v>38</v>
+      </c>
+      <c r="B19" t="s" s="13">
+        <v>39</v>
+      </c>
+      <c r="C19" t="s" s="15">
+        <v>35</v>
+      </c>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="17"/>
     </row>
     <row r="20" ht="53.25" customHeight="1">
       <c r="A20" t="s" s="13">
-        <v>25</v>
-      </c>
-      <c r="B20" s="14">
-        <v>43118</v>
-      </c>
-      <c r="C20" t="s" s="16">
-        <v>28</v>
-      </c>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="18"/>
+        <v>40</v>
+      </c>
+      <c r="B20" t="s" s="13">
+        <v>41</v>
+      </c>
+      <c r="C20" t="s" s="15">
+        <v>35</v>
+      </c>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="17"/>
     </row>
     <row r="21" ht="49.5" customHeight="1">
       <c r="A21" t="s" s="13">
-        <v>26</v>
-      </c>
-      <c r="B21" s="14">
-        <v>43119</v>
-      </c>
-      <c r="C21" t="s" s="16">
-        <v>28</v>
-      </c>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="18"/>
+        <v>42</v>
+      </c>
+      <c r="B21" t="s" s="13">
+        <v>43</v>
+      </c>
+      <c r="C21" t="s" s="15">
+        <v>35</v>
+      </c>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="17"/>
     </row>
     <row r="22" ht="30.75" customHeight="1">
       <c r="A22" t="s" s="13">
-        <v>29</v>
-      </c>
-      <c r="B22" s="19"/>
-      <c r="C22" s="20"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="18"/>
+        <v>44</v>
+      </c>
+      <c r="B22" s="18"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="17"/>
     </row>
     <row r="23" ht="98.25" customHeight="1">
-      <c r="A23" t="s" s="21">
-        <v>30</v>
-      </c>
-      <c r="B23" s="22"/>
-      <c r="C23" s="22"/>
-      <c r="D23" s="22"/>
-      <c r="E23" s="22"/>
-      <c r="F23" s="22"/>
+      <c r="A23" t="s" s="20">
+        <v>45</v>
+      </c>
+      <c r="B23" s="21"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="27">

</xml_diff>

<commit_message>
feat(module) : replace time
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -124,11 +124,11 @@
     <t>新项目后台数据及逻辑交互</t>
   </si>
   <si>
-    <t xml:space="preserve">{nextWeek.Thes}
+    <t xml:space="preserve">{nextWeek.Tues}
 </t>
   </si>
   <si>
-    <t xml:space="preserve">{nextWeek.ThesDate}
+    <t xml:space="preserve">{nextWeek.TuesDate}
 </t>
   </si>
   <si>
@@ -1803,33 +1803,33 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="A15:F15"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="A23:F23"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="C22:F22"/>
+    <mergeCell ref="C19:F19"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="C18:F18"/>
+    <mergeCell ref="C21:F21"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="C17:F17"/>
     <mergeCell ref="C20:F20"/>
-    <mergeCell ref="C17:F17"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="C21:F21"/>
-    <mergeCell ref="C18:F18"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="C19:F19"/>
-    <mergeCell ref="C22:F22"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="A23:F23"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="C16:F16"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="A15:F15"/>
-    <mergeCell ref="D3:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>

<commit_message>
feat(module) : add rules
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="55">
   <si>
     <t>{position}周报（{month}月）</t>
   </si>
@@ -87,28 +87,43 @@
 </t>
   </si>
   <si>
+    <t>{thisWeekdo1}</t>
+  </si>
+  <si>
     <t>{thisWeek.Tues}</t>
   </si>
   <si>
     <t>{thisWeek.TuesDate}</t>
   </si>
   <si>
+    <t>{thisWeekdo2}</t>
+  </si>
+  <si>
     <t>{thisWeek.Wed}</t>
   </si>
   <si>
     <t>{thisWeek.WedDate}</t>
   </si>
   <si>
+    <t>{thisWeekdo3}</t>
+  </si>
+  <si>
     <t>{thisWeek.Thur}</t>
   </si>
   <si>
     <t>{thisWeek.ThurDate}</t>
   </si>
   <si>
+    <t>{thisWeekdo4}</t>
+  </si>
+  <si>
     <t>{thisWeek.Fri}</t>
   </si>
   <si>
     <t>{thisWeek.FriDate}</t>
+  </si>
+  <si>
+    <t>{thisWeekdo5}</t>
   </si>
   <si>
     <t>下周工作计划</t>
@@ -121,7 +136,7 @@
     <t>{nextWeek.MonDate}</t>
   </si>
   <si>
-    <t>新项目后台数据及逻辑交互</t>
+    <t>{nextWeekdo1}</t>
   </si>
   <si>
     <t xml:space="preserve">{nextWeek.Tues}
@@ -132,6 +147,9 @@
 </t>
   </si>
   <si>
+    <t>{nextWeekdo2}</t>
+  </si>
+  <si>
     <t xml:space="preserve">{nextWeek.Wed}
 </t>
   </si>
@@ -140,6 +158,9 @@
 </t>
   </si>
   <si>
+    <t>{nextWeekdo3}</t>
+  </si>
+  <si>
     <t xml:space="preserve">{nextWeek.Thur}
 </t>
   </si>
@@ -148,6 +169,9 @@
 </t>
   </si>
   <si>
+    <t>{nextWeekdo4}</t>
+  </si>
+  <si>
     <t xml:space="preserve">{nextWeek.Fri}
 </t>
   </si>
@@ -156,10 +180,13 @@
 </t>
   </si>
   <si>
+    <t>{nextWeekdo5}</t>
+  </si>
+  <si>
     <t>额外工作说明</t>
   </si>
   <si>
-    <t>本周工作总结：项目理解,优化,开发</t>
+    <t>本周工作总结：{summer}</t>
   </si>
 </sst>
 </file>
@@ -1630,7 +1657,9 @@
       <c r="B10" t="s" s="13">
         <v>23</v>
       </c>
-      <c r="C10" s="12"/>
+      <c r="C10" t="s" s="11">
+        <v>24</v>
+      </c>
       <c r="D10" s="10">
         <v>1</v>
       </c>
@@ -1639,12 +1668,14 @@
     </row>
     <row r="11" ht="59.25" customHeight="1">
       <c r="A11" t="s" s="13">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B11" t="s" s="13">
-        <v>25</v>
-      </c>
-      <c r="C11" s="12"/>
+        <v>26</v>
+      </c>
+      <c r="C11" t="s" s="11">
+        <v>27</v>
+      </c>
       <c r="D11" s="10">
         <v>2</v>
       </c>
@@ -1653,12 +1684,14 @@
     </row>
     <row r="12" ht="51.75" customHeight="1">
       <c r="A12" t="s" s="13">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B12" t="s" s="13">
-        <v>27</v>
-      </c>
-      <c r="C12" s="12"/>
+        <v>29</v>
+      </c>
+      <c r="C12" t="s" s="11">
+        <v>30</v>
+      </c>
       <c r="D12" s="10">
         <v>3</v>
       </c>
@@ -1667,31 +1700,35 @@
     </row>
     <row r="13" ht="51.75" customHeight="1">
       <c r="A13" t="s" s="13">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B13" t="s" s="13">
-        <v>29</v>
-      </c>
-      <c r="C13" s="12"/>
+        <v>32</v>
+      </c>
+      <c r="C13" t="s" s="11">
+        <v>33</v>
+      </c>
       <c r="D13" s="14"/>
       <c r="E13" s="12"/>
       <c r="F13" s="12"/>
     </row>
     <row r="14" ht="59.25" customHeight="1">
       <c r="A14" t="s" s="13">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B14" t="s" s="13">
-        <v>31</v>
-      </c>
-      <c r="C14" s="12"/>
+        <v>35</v>
+      </c>
+      <c r="C14" t="s" s="11">
+        <v>36</v>
+      </c>
       <c r="D14" s="14"/>
       <c r="E14" s="12"/>
       <c r="F14" s="12"/>
     </row>
     <row r="15" ht="26" customHeight="1">
       <c r="A15" t="s" s="6">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
@@ -1713,13 +1750,13 @@
     </row>
     <row r="17" ht="57" customHeight="1">
       <c r="A17" t="s" s="13">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B17" t="s" s="13">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C17" t="s" s="15">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="D17" s="16"/>
       <c r="E17" s="16"/>
@@ -1727,13 +1764,13 @@
     </row>
     <row r="18" ht="51" customHeight="1">
       <c r="A18" t="s" s="13">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B18" t="s" s="13">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C18" t="s" s="15">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="D18" s="16"/>
       <c r="E18" s="16"/>
@@ -1741,13 +1778,13 @@
     </row>
     <row r="19" ht="53.25" customHeight="1">
       <c r="A19" t="s" s="13">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="B19" t="s" s="13">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="C19" t="s" s="15">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="D19" s="16"/>
       <c r="E19" s="16"/>
@@ -1755,13 +1792,13 @@
     </row>
     <row r="20" ht="53.25" customHeight="1">
       <c r="A20" t="s" s="13">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="B20" t="s" s="13">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="C20" t="s" s="15">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="D20" s="16"/>
       <c r="E20" s="16"/>
@@ -1769,13 +1806,13 @@
     </row>
     <row r="21" ht="49.5" customHeight="1">
       <c r="A21" t="s" s="13">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="B21" t="s" s="13">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="C21" t="s" s="15">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="D21" s="16"/>
       <c r="E21" s="16"/>
@@ -1783,7 +1820,7 @@
     </row>
     <row r="22" ht="30.75" customHeight="1">
       <c r="A22" t="s" s="13">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="B22" s="18"/>
       <c r="C22" s="19"/>
@@ -1793,7 +1830,7 @@
     </row>
     <row r="23" ht="98.25" customHeight="1">
       <c r="A23" t="s" s="20">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="B23" s="21"/>
       <c r="C23" s="21"/>
@@ -1803,33 +1840,33 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="C20:F20"/>
+    <mergeCell ref="C17:F17"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="C21:F21"/>
+    <mergeCell ref="C18:F18"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="C19:F19"/>
+    <mergeCell ref="C22:F22"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="A23:F23"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="A15:F15"/>
     <mergeCell ref="D3:F3"/>
-    <mergeCell ref="A15:F15"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="C16:F16"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="A23:F23"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="C22:F22"/>
-    <mergeCell ref="C19:F19"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="C18:F18"/>
-    <mergeCell ref="C21:F21"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="C17:F17"/>
-    <mergeCell ref="C20:F20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>